<commit_message>
Edit government revenue accounting assumptions for carbon tax
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/GRA/Government Revenue Accounting.xlsx
+++ b/InputData/ctrl-settings/GRA/Government Revenue Accounting.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\ctrl-settings\GRA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\ctrl-settings\GRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89927AC9-6C74-4B96-B011-B1F3D3363FD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="2670" windowWidth="25665" windowHeight="13515" tabRatio="698" xr2:uid="{26206BE0-D423-40C5-BC54-AB75C15D3AEF}"/>
+    <workbookView xWindow="2070" yWindow="2670" windowWidth="25665" windowHeight="13515" tabRatio="698"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
     <sheet name="GRA-ntnldebtinterest" sheetId="15" r:id="rId10"/>
     <sheet name="GRA-remainder" sheetId="16" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,17 +42,26 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={4F81BCB5-E56D-426A-91DB-BCF0877CB817}</author>
   </authors>
   <commentList>
-    <comment ref="C15" authorId="0" shapeId="0" xr:uid="{4F81BCB5-E56D-426A-91DB-BCF0877CB817}">
+    <comment ref="C15" authorId="0" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     It is recommended to leave this cell set to zero and to set a non-zero value in at least one other cell in this row.</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -264,8 +272,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,12 +312,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -711,22 +713,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3857EE15-0702-4D02-88A1-477DCCE329DB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="80.85546875" customWidth="1"/>
+    <col min="2" max="2" width="80.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -734,72 +736,72 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
         <v>1</v>
       </c>
@@ -807,7 +809,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
         <v>2</v>
       </c>
@@ -815,7 +817,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
         <v>3</v>
       </c>
@@ -823,7 +825,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
         <v>4</v>
       </c>
@@ -831,7 +833,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
         <v>5</v>
       </c>
@@ -839,114 +841,114 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B26" s="5"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" s="12" t="s">
         <v>55</v>
       </c>
       <c r="B41" s="13"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>63</v>
       </c>
@@ -958,7 +960,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B57F2C9C-1694-4A27-BF05-C8B0A1B522A6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
@@ -966,12 +968,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -979,7 +981,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -988,7 +990,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -996,7 +998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1004,7 +1006,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1012,7 +1014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1026,7 +1028,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{521CDC7A-C360-4D48-B6EF-82826DA4B3B6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1034,12 +1036,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1047,7 +1049,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1056,7 +1058,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1064,7 +1066,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1072,7 +1074,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1080,7 +1082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1094,41 +1096,43 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC2A49CB-6D0E-4B96-B95B-51D10E021D04}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
     <col min="2" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="8" t="s">
         <v>51</v>
       </c>
@@ -1138,7 +1142,7 @@
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>46</v>
       </c>
@@ -1158,7 +1162,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -1166,19 +1170,19 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <v>5</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1198,7 +1202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1218,7 +1222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1238,7 +1242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1258,7 +1262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1278,7 +1282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1298,7 +1302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1318,7 +1322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1338,7 +1342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="12" t="s">
         <v>52</v>
       </c>
@@ -1348,12 +1352,12 @@
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
         <v>46</v>
       </c>
@@ -1373,7 +1377,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -1383,22 +1387,22 @@
       </c>
       <c r="C22" s="10">
         <f t="shared" ref="C22:F22" si="0">IFERROR(C8/SUM($B8:$F8),1/COUNT($B8:$F8))</f>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D22" s="10">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E22" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F22" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -1423,7 +1427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -1448,7 +1452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -1473,7 +1477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -1498,7 +1502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -1523,7 +1527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -1548,7 +1552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -1573,7 +1577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1606,7 +1610,77 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42AF1F77-591B-419B-91FC-2618E46BD93A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="4" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="34.86328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2">
+        <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B8:F8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1614,29 +1688,29 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>47</v>
       </c>
       <c r="B2">
-        <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B8:F8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B9:F9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1644,7 +1718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1652,7 +1726,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1660,7 +1734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1673,8 +1747,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A3C2F6F-98F7-47BF-A121-519530665716}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1682,45 +1756,45 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>47</v>
       </c>
       <c r="B2">
-        <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B9:F9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B10:F10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>48</v>
       </c>
       <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>49</v>
       </c>
       <c r="B4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1728,7 +1802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1741,8 +1815,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E95D8AB2-6798-43D7-AB4D-CF9027D5D76D}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1750,29 +1824,29 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>47</v>
       </c>
       <c r="B2">
-        <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B10:F10)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B11:F11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1780,7 +1854,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1788,7 +1862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1796,7 +1870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1809,8 +1883,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB851FAA-54C9-43D6-9286-3EB2FEDE6F50}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1818,29 +1892,29 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>47</v>
       </c>
       <c r="B2">
-        <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B11:F11)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B12:F12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1848,7 +1922,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1856,7 +1930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1864,7 +1938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1877,8 +1951,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41A3B53A-6256-48D4-9FF6-54DB202AB422}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1886,29 +1960,29 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>47</v>
       </c>
       <c r="B2">
-        <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B12:F12)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B13:F13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1916,7 +1990,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1924,7 +1998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1932,7 +2006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1945,8 +2019,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1EB629B-80DD-4A77-AF4C-E5418F20EE0D}">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1954,29 +2028,29 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>47</v>
       </c>
       <c r="B2">
-        <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B13:F13)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B14:F14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1984,7 +2058,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1992,7 +2066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -2000,75 +2074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85184EB0-77F4-492B-91CC-4F8870FED453}">
-  <sheetPr>
-    <tabColor theme="4" tint="-0.249977111117893"/>
-  </sheetPr>
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2">
-        <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B14:F14)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
Change default fuel tax revenue GRA setting
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/GRA/Government Revenue Accounting.xlsx
+++ b/InputData/ctrl-settings/GRA/Government Revenue Accounting.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\ctrl-settings\GRA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-us\InputData\ctrl-settings\GRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1103,7 +1103,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1190,16 +1190,16 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
@@ -1412,11 +1412,11 @@
       </c>
       <c r="C23" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D23" s="10">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" s="10">
         <f t="shared" si="1"/>
@@ -1424,7 +1424,7 @@
       </c>
       <c r="F23" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
@@ -1686,7 +1686,9 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1715,7 +1717,7 @@
         <v>48</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
@@ -1723,7 +1725,7 @@
         <v>49</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
@@ -1739,7 +1741,7 @@
         <v>64</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change name of battery production subsidy cash flow subscript, add grid battery production subsidies into proper GRA category, add missing government cash flow types to output graph
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/GRA/Government Revenue Accounting.xlsx
+++ b/InputData/ctrl-settings/GRA/Government Revenue Accounting.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\ctrl-settings\GRA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\ctrl-settings\GRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D819826-0E41-444E-85CC-5113AD7B4B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7CE58D-EFCE-4C47-AC59-CD90A508527F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="698" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" tabRatio="698" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="GRA-carbontax" sheetId="8" r:id="rId3"/>
     <sheet name="GRA-fueltax" sheetId="9" r:id="rId4"/>
     <sheet name="GRA-evsubsidy" sheetId="10" r:id="rId5"/>
-    <sheet name="GRA-vehbatsubsidy" sheetId="18" r:id="rId6"/>
+    <sheet name="GRA-batconsubsidy" sheetId="18" r:id="rId6"/>
     <sheet name="GRA-elecgensubsidy" sheetId="11" r:id="rId7"/>
     <sheet name="GRA-eleccapconstsubsidy" sheetId="12" r:id="rId8"/>
     <sheet name="GRA-distsolarsubsidy" sheetId="13" r:id="rId9"/>
@@ -407,9 +407,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -447,7 +447,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -553,7 +553,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -695,7 +695,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -715,17 +715,17 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="80.85546875" customWidth="1"/>
+    <col min="2" max="2" width="80.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -733,72 +733,72 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>1</v>
       </c>
@@ -806,7 +806,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>2</v>
       </c>
@@ -814,7 +814,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>3</v>
       </c>
@@ -822,7 +822,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>4</v>
       </c>
@@ -830,7 +830,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>5</v>
       </c>
@@ -838,114 +838,114 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B26" s="5"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="12" t="s">
         <v>55</v>
       </c>
       <c r="B41" s="13"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>63</v>
       </c>
@@ -967,12 +967,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -980,7 +980,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -989,7 +989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -997,7 +997,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1037,12 +1037,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1105,12 +1105,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1173,12 +1173,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1243,33 +1243,33 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
     <col min="2" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>51</v>
       </c>
@@ -1279,7 +1279,7 @@
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>46</v>
       </c>
@@ -1299,7 +1299,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1359,7 +1359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
         <v>52</v>
       </c>
@@ -1489,12 +1489,12 @@
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>46</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1757,12 +1757,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1770,7 +1770,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1827,12 +1827,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1895,12 +1895,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1962,15 +1962,15 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1987,7 +1987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -2033,12 +2033,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -2101,12 +2101,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -2114,7 +2114,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -2169,12 +2169,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -2191,7 +2191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>

</xml_diff>